<commit_message>
099 ____ extraRegels aangepast
</commit_message>
<xml_diff>
--- a/uml/IMKL2015 v 099-object-attributen-ExtraRegels.xlsx
+++ b/uml/IMKL2015 v 099-object-attributen-ExtraRegels.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20400" windowHeight="8325" tabRatio="875" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20400" windowHeight="8325" tabRatio="875" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL2.2ExtraRegels" sheetId="23" state="hidden" r:id="rId1"/>
@@ -4181,7 +4181,7 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -14496,7 +14496,7 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>

</xml_diff>